<commit_message>
chore: 생산 현황 template - 전극 - 조립 - 화성
</commit_message>
<xml_diff>
--- a/data/templates/status/assembly.xlsx
+++ b/data/templates/status/assembly.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\eurocell-mes-be\data\templates\status\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D92EC75-8B88-488C-BCBB-F3A883882B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5F80F2-8520-405A-A897-46752E677F6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E25BFB65-D502-4278-AB85-8965F34E216B}"/>
+    <workbookView xWindow="1065" yWindow="120" windowWidth="25575" windowHeight="15210" xr2:uid="{E25BFB65-D502-4278-AB85-8965F34E216B}"/>
   </bookViews>
   <sheets>
     <sheet name="조립 공정" sheetId="1" r:id="rId1"/>
@@ -387,7 +387,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -415,6 +415,27 @@
     <xf numFmtId="176" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -433,6 +454,42 @@
     <xf numFmtId="9" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -451,6 +508,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -460,79 +523,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -872,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA69F4FE-7083-4A74-91FA-43A59943F702}">
   <dimension ref="A1:AL48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AO20" sqref="AN20:AO20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AI49" sqref="AI49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -889,11 +886,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="20"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="39"/>
       <c r="D1" s="2">
         <v>1</v>
       </c>
@@ -1001,13 +998,13 @@
       </c>
     </row>
     <row r="2" spans="1:38" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="31" t="s">
         <v>0</v>
       </c>
       <c r="D2" s="7"/>
@@ -1045,19 +1042,19 @@
         <f>SUM(D2:AH2)</f>
         <v>0</v>
       </c>
-      <c r="AJ2" s="46"/>
-      <c r="AK2" s="47" t="str">
+      <c r="AJ2" s="30"/>
+      <c r="AK2" s="22" t="str">
         <f t="shared" ref="AK2" si="0">IFERROR(AI2/AL2,"")</f>
         <v/>
       </c>
-      <c r="AL2" s="46"/>
+      <c r="AL2" s="30"/>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A3" s="33"/>
-      <c r="B3" s="36" t="s">
+      <c r="A3" s="40"/>
+      <c r="B3" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="35"/>
+      <c r="C3" s="31"/>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -1093,16 +1090,16 @@
         <f t="shared" ref="AI3:AI26" si="1">SUM(D3:AH3)</f>
         <v>0</v>
       </c>
-      <c r="AJ3" s="46"/>
-      <c r="AK3" s="47"/>
-      <c r="AL3" s="46"/>
+      <c r="AJ3" s="30"/>
+      <c r="AK3" s="22"/>
+      <c r="AL3" s="30"/>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A4" s="33"/>
-      <c r="B4" s="37" t="s">
+      <c r="A4" s="40"/>
+      <c r="B4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="35"/>
+      <c r="C4" s="31"/>
       <c r="D4" s="4" t="str">
         <f>IFERROR(D2/(D2+D3),"")</f>
         <v/>
@@ -1231,16 +1228,16 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="AJ4" s="46"/>
-      <c r="AK4" s="47"/>
-      <c r="AL4" s="46"/>
+      <c r="AJ4" s="30"/>
+      <c r="AK4" s="22"/>
+      <c r="AL4" s="30"/>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A5" s="33"/>
-      <c r="B5" s="34" t="s">
+      <c r="A5" s="40"/>
+      <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="32" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="7"/>
@@ -1278,19 +1275,19 @@
         <f>SUM(D5:AH5)</f>
         <v>0</v>
       </c>
-      <c r="AJ5" s="48"/>
-      <c r="AK5" s="12" t="str">
+      <c r="AJ5" s="33"/>
+      <c r="AK5" s="19" t="str">
         <f t="shared" ref="AK5" si="3">IFERROR(AI5/AL5,"")</f>
         <v/>
       </c>
-      <c r="AL5" s="9"/>
+      <c r="AL5" s="16"/>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A6" s="33"/>
-      <c r="B6" s="36" t="s">
+      <c r="A6" s="40"/>
+      <c r="B6" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="38"/>
+      <c r="C6" s="32"/>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -1326,16 +1323,16 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ6" s="48"/>
-      <c r="AK6" s="13"/>
-      <c r="AL6" s="10"/>
+      <c r="AJ6" s="33"/>
+      <c r="AK6" s="20"/>
+      <c r="AL6" s="17"/>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A7" s="33"/>
-      <c r="B7" s="37" t="s">
+      <c r="A7" s="40"/>
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="38"/>
+      <c r="C7" s="32"/>
       <c r="D7" s="4" t="str">
         <f>IFERROR(D5/(D5+D6),"")</f>
         <v/>
@@ -1464,18 +1461,18 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="AJ7" s="48"/>
-      <c r="AK7" s="14"/>
-      <c r="AL7" s="11"/>
+      <c r="AJ7" s="33"/>
+      <c r="AK7" s="21"/>
+      <c r="AL7" s="18"/>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A8" s="39" t="s">
+      <c r="A8" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="14" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="7"/>
@@ -1510,20 +1507,20 @@
       <c r="AG8" s="7"/>
       <c r="AH8" s="7"/>
       <c r="AI8" s="8">
-        <f t="shared" si="1"/>
+        <f>SUM(D8:AH8)</f>
         <v>0</v>
       </c>
-      <c r="AJ8" s="9"/>
-      <c r="AK8" s="12" t="str">
+      <c r="AJ8" s="16"/>
+      <c r="AK8" s="19" t="str">
         <f>IFERROR(AI11/AL8,"")</f>
         <v/>
       </c>
-      <c r="AL8" s="9"/>
+      <c r="AL8" s="16"/>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="31" t="s">
+      <c r="A9" s="41"/>
+      <c r="B9" s="43"/>
+      <c r="C9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="7"/>
@@ -1561,152 +1558,149 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ9" s="10"/>
-      <c r="AK9" s="13"/>
-      <c r="AL9" s="10"/>
+      <c r="AJ9" s="17"/>
+      <c r="AK9" s="20"/>
+      <c r="AL9" s="17"/>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="31" t="s">
+      <c r="A10" s="41"/>
+      <c r="B10" s="43"/>
+      <c r="C10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D10" s="45" t="str">
-        <f t="shared" ref="D7:AI26" si="5">IFERROR(D8/(D8+D9),"")</f>
-        <v/>
-      </c>
-      <c r="E10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="G10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="H10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="J10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="K10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="L10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="M10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="O10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="R10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="S10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="U10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="V10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="W10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="X10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Y10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Z10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AA10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AB10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AC10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AD10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AE10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AF10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AG10" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AH10" s="45" t="str">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="str">
+        <f t="shared" ref="D10:AH26" si="5">IFERROR(E8/(E8+E9),"")</f>
+        <v/>
+      </c>
+      <c r="F10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="H10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="T10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="U10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="V10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="W10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Z10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AA10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AB10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AC10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AD10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AE10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AF10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AG10" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AH10" s="7" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="AI10" s="8">
-        <f t="shared" si="1"/>
+        <f>SUM(D10:AH10)</f>
         <v>0</v>
       </c>
-      <c r="AJ10" s="10"/>
-      <c r="AK10" s="13"/>
-      <c r="AL10" s="10"/>
+      <c r="AJ10" s="17"/>
+      <c r="AK10" s="20"/>
+      <c r="AL10" s="17"/>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="41" t="s">
+      <c r="A11" s="41"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D11" s="7"/>
@@ -1744,19 +1738,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ11" s="10"/>
-      <c r="AK11" s="13" t="str">
-        <f t="shared" ref="AK8:AK16" si="6">IFERROR(AI11/AL11,"")</f>
-        <v/>
-      </c>
-      <c r="AL11" s="10"/>
+      <c r="AJ11" s="17"/>
+      <c r="AK11" s="20" t="str">
+        <f t="shared" ref="AK11:AK14" si="6">IFERROR(AI11/AL11,"")</f>
+        <v/>
+      </c>
+      <c r="AL11" s="17"/>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
-      <c r="B12" s="25" t="s">
+      <c r="A12" s="41"/>
+      <c r="B12" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="15" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="7"/>
@@ -1794,14 +1788,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ12" s="10"/>
-      <c r="AK12" s="13"/>
-      <c r="AL12" s="10"/>
+      <c r="AJ12" s="17"/>
+      <c r="AK12" s="20"/>
+      <c r="AL12" s="17"/>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="31" t="s">
+      <c r="A13" s="41"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="9" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="7"/>
@@ -1839,14 +1833,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ13" s="10"/>
-      <c r="AK13" s="13"/>
-      <c r="AL13" s="10"/>
+      <c r="AJ13" s="17"/>
+      <c r="AK13" s="20"/>
+      <c r="AL13" s="17"/>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A14" s="39"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="31" t="s">
+      <c r="A14" s="41"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="7"/>
@@ -1884,17 +1878,17 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ14" s="10"/>
-      <c r="AK14" s="13" t="str">
+      <c r="AJ14" s="17"/>
+      <c r="AK14" s="20" t="str">
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AL14" s="10"/>
+      <c r="AL14" s="17"/>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A15" s="39"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="41" t="s">
+      <c r="A15" s="41"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="15" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="7"/>
@@ -1932,22 +1926,22 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ15" s="10"/>
-      <c r="AK15" s="13"/>
-      <c r="AL15" s="10"/>
+      <c r="AJ15" s="17"/>
+      <c r="AK15" s="20"/>
+      <c r="AL15" s="17"/>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A16" s="39"/>
-      <c r="B16" s="42" t="s">
+      <c r="A16" s="41"/>
+      <c r="B16" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="42"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="4" t="str">
-        <f>IFERROR(D14/(D14+D15),"")</f>
+        <f t="shared" ref="D16:P16" si="7">IF(SUM(B8:B11)=0,"",IFERROR((IF(B11&lt;&gt;"",B11-IF(B15="",0,B15),IF(B10&lt;&gt;"",B10-IF(B14="",0,B14),IF(B9&lt;&gt;"",B9-IF(B13="",0,B13),B8-IF(B12="",0,B12)))))/(IF(B8&lt;&gt;"",B8,IF(B9&lt;&gt;"",B9,IF(B10&lt;&gt;"",B10,B11)))),""))</f>
         <v/>
       </c>
       <c r="E16" s="4" t="str">
-        <f t="shared" ref="E16:AI16" si="7">IFERROR(E14/(E14+E15),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="F16" s="4" t="str">
@@ -1995,93 +1989,93 @@
         <v/>
       </c>
       <c r="Q16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(SUM(O8:O11)=0,"",IFERROR((IF(O11&lt;&gt;"",O11-IF(O15="",0,O15),IF(O10&lt;&gt;"",O10-IF(O14="",0,O14),IF(O9&lt;&gt;"",O9-IF(O13="",0,O13),O8-IF(O12="",0,O12)))))/(IF(O8&lt;&gt;"",O8,IF(O9&lt;&gt;"",O9,IF(O10&lt;&gt;"",O10,O11)))),""))</f>
         <v/>
       </c>
       <c r="R16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" ref="R16:AH16" si="8">IF(SUM(P8:P11)=0,"",IFERROR((IF(P11&lt;&gt;"",P11-IF(P15="",0,P15),IF(P10&lt;&gt;"",P10-IF(P14="",0,P14),IF(P9&lt;&gt;"",P9-IF(P13="",0,P13),P8-IF(P12="",0,P12)))))/(IF(P8&lt;&gt;"",P8,IF(P9&lt;&gt;"",P9,IF(P10&lt;&gt;"",P10,P11)))),""))</f>
         <v/>
       </c>
       <c r="S16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="T16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="U16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="V16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="W16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="X16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="Y16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="Z16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AA16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AB16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AC16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AD16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AE16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AF16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AG16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AH16" s="4" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="AI16" s="4" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="AJ16" s="11"/>
-      <c r="AK16" s="14"/>
-      <c r="AL16" s="11"/>
+        <f>IFERROR((AI11-AI15)/AI8,"")</f>
+        <v/>
+      </c>
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="21"/>
+      <c r="AL16" s="18"/>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A17" s="39" t="s">
+      <c r="A17" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="35"/>
+      <c r="C17" s="31"/>
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -2117,19 +2111,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ17" s="25"/>
-      <c r="AK17" s="12" t="str">
+      <c r="AJ17" s="23"/>
+      <c r="AK17" s="19" t="str">
         <f>IFERROR(AI17/AL17,"")</f>
         <v/>
       </c>
-      <c r="AL17" s="9"/>
+      <c r="AL17" s="16"/>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A18" s="39"/>
-      <c r="B18" s="43" t="s">
+      <c r="A18" s="41"/>
+      <c r="B18" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="43"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -2165,139 +2159,139 @@
         <f>SUM(D18:AH18)</f>
         <v>0</v>
       </c>
-      <c r="AJ18" s="26"/>
-      <c r="AK18" s="13"/>
-      <c r="AL18" s="10"/>
+      <c r="AJ18" s="24"/>
+      <c r="AK18" s="20"/>
+      <c r="AL18" s="17"/>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A19" s="39"/>
-      <c r="B19" s="43" t="s">
+      <c r="A19" s="41"/>
+      <c r="B19" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="44" t="s">
+      <c r="C19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="G19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="H19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="J19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="K19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="L19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="M19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="O19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="R19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="S19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="U19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="V19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="W19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="X19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Y19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Z19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AA19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AB19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AC19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AD19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AE19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AF19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AG19" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AH19" s="45" t="str">
+      <c r="D19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="H19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="T19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="U19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="V19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="W19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Z19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AA19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AB19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AC19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AD19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AE19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AF19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AG19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AH19" s="7" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
@@ -2305,14 +2299,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ19" s="26"/>
-      <c r="AK19" s="13"/>
-      <c r="AL19" s="10"/>
+      <c r="AJ19" s="24"/>
+      <c r="AK19" s="20"/>
+      <c r="AL19" s="17"/>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A20" s="39"/>
-      <c r="B20" s="43"/>
-      <c r="C20" s="41" t="s">
+      <c r="A20" s="41"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="15" t="s">
         <v>21</v>
       </c>
       <c r="D20" s="7"/>
@@ -2350,14 +2344,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ20" s="26"/>
-      <c r="AK20" s="13"/>
-      <c r="AL20" s="10"/>
+      <c r="AJ20" s="24"/>
+      <c r="AK20" s="20"/>
+      <c r="AL20" s="17"/>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A21" s="39"/>
-      <c r="B21" s="43"/>
-      <c r="C21" s="41" t="s">
+      <c r="A21" s="41"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="15" t="s">
         <v>22</v>
       </c>
       <c r="D21" s="7"/>
@@ -2395,14 +2389,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ21" s="26"/>
-      <c r="AK21" s="13"/>
-      <c r="AL21" s="10"/>
+      <c r="AJ21" s="24"/>
+      <c r="AK21" s="20"/>
+      <c r="AL21" s="17"/>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A22" s="39"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="36" t="s">
+      <c r="A22" s="41"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="11" t="s">
         <v>23</v>
       </c>
       <c r="D22" s="7"/>
@@ -2440,156 +2434,156 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ22" s="26"/>
-      <c r="AK22" s="13"/>
-      <c r="AL22" s="10"/>
+      <c r="AJ22" s="24"/>
+      <c r="AK22" s="20"/>
+      <c r="AL22" s="17"/>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A23" s="39"/>
-      <c r="B23" s="42" t="s">
+      <c r="A23" s="41"/>
+      <c r="B23" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="42"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="4" t="str">
-        <f>IFERROR(D21/(D21+D22),"")</f>
+        <f>IFERROR(D17/(D17+D18),"")</f>
         <v/>
       </c>
       <c r="E23" s="4" t="str">
-        <f t="shared" ref="E23:AI23" si="8">IFERROR(E21/(E21+E22),"")</f>
+        <f t="shared" ref="E23:AH23" si="9">IFERROR(E17/(E17+E18),"")</f>
         <v/>
       </c>
       <c r="F23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="H23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="I23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="J23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="K23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="L23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="N23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="O23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="P23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="Q23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="R23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="S23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="T23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="U23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="V23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="W23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="X23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="Y23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="Z23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AA23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AB23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AC23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AD23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AE23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AF23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AG23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AH23" s="4" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="AI23" s="4" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AJ23" s="27"/>
-      <c r="AK23" s="14"/>
-      <c r="AL23" s="11"/>
+        <f>IFERROR(AI17/(AI17+AI18),"")</f>
+        <v/>
+      </c>
+      <c r="AJ23" s="25"/>
+      <c r="AK23" s="21"/>
+      <c r="AL23" s="18"/>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="B24" s="35" t="s">
+      <c r="B24" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="35"/>
+      <c r="C24" s="31"/>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -2625,19 +2619,19 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ24" s="9"/>
-      <c r="AK24" s="12" t="str">
-        <f t="shared" ref="AK24:AK29" si="9">IFERROR(AI24/AL24,"")</f>
-        <v/>
-      </c>
-      <c r="AL24" s="9"/>
+      <c r="AJ24" s="16"/>
+      <c r="AK24" s="19" t="str">
+        <f t="shared" ref="AK24:AK27" si="10">IFERROR(AI24/AL24,"")</f>
+        <v/>
+      </c>
+      <c r="AL24" s="16"/>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A25" s="29"/>
-      <c r="B25" s="24" t="s">
+      <c r="A25" s="46"/>
+      <c r="B25" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="27"/>
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -2673,139 +2667,139 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ25" s="10"/>
-      <c r="AK25" s="13"/>
-      <c r="AL25" s="10"/>
+      <c r="AJ25" s="17"/>
+      <c r="AK25" s="20"/>
+      <c r="AL25" s="17"/>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A26" s="29"/>
-      <c r="B26" s="43" t="s">
+      <c r="A26" s="46"/>
+      <c r="B26" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C26" s="44" t="s">
+      <c r="C26" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="E26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="F26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="G26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="H26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="I26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="J26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="K26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="L26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="M26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="N26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="O26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="P26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Q26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="R26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="S26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="T26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="U26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="V26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="W26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="X26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Y26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="Z26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AA26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AB26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AC26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AD26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AE26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AF26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AG26" s="45" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-      <c r="AH26" s="45" t="str">
+      <c r="D26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="E26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="F26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="G26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="H26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="J26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="K26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="L26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="M26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="N26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="O26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="P26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Q26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="R26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="S26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="T26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="U26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="V26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="W26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="X26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Y26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="Z26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AA26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AB26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AC26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AD26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AE26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AF26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AG26" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="AH26" s="7" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
@@ -2813,14 +2807,14 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AJ26" s="10"/>
-      <c r="AK26" s="13"/>
-      <c r="AL26" s="10"/>
+      <c r="AJ26" s="17"/>
+      <c r="AK26" s="20"/>
+      <c r="AL26" s="17"/>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A27" s="29"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="34" t="s">
+      <c r="A27" s="46"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="10" t="s">
         <v>29</v>
       </c>
       <c r="D27" s="7"/>
@@ -2855,20 +2849,20 @@
       <c r="AG27" s="7"/>
       <c r="AH27" s="7"/>
       <c r="AI27" s="8">
-        <f t="shared" ref="AI27:AI28" si="10">SUM(D27:AH27)</f>
+        <f t="shared" ref="AI27:AI28" si="11">SUM(D27:AH27)</f>
         <v>0</v>
       </c>
-      <c r="AJ27" s="10"/>
-      <c r="AK27" s="13" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="AL27" s="10"/>
+      <c r="AJ27" s="17"/>
+      <c r="AK27" s="20" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
+      <c r="AL27" s="17"/>
     </row>
     <row r="28" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A28" s="29"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="36" t="s">
+      <c r="A28" s="46"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="11" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="7"/>
@@ -2903,1034 +2897,1034 @@
       <c r="AG28" s="7"/>
       <c r="AH28" s="7"/>
       <c r="AI28" s="8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AJ28" s="10"/>
-      <c r="AK28" s="13"/>
-      <c r="AL28" s="10"/>
+      <c r="AJ28" s="17"/>
+      <c r="AK28" s="20"/>
+      <c r="AL28" s="17"/>
     </row>
     <row r="29" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A29" s="29"/>
-      <c r="B29" s="42" t="s">
+      <c r="A29" s="46"/>
+      <c r="B29" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="42"/>
+      <c r="C29" s="28"/>
       <c r="D29" s="4" t="str">
-        <f>IFERROR(D27/(D27+D28),"")</f>
+        <f>IFERROR(D24/(D24+D25),"")</f>
         <v/>
       </c>
       <c r="E29" s="4" t="str">
-        <f t="shared" ref="E29:AI29" si="11">IFERROR(E27/(E27+E28),"")</f>
+        <f t="shared" ref="E29:AH29" si="12">IFERROR(E24/(E24+E25),"")</f>
         <v/>
       </c>
       <c r="F29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="G29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="H29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="I29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="J29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="K29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="L29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="M29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="N29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="O29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="P29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="Q29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="R29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="S29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="T29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="U29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="V29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="W29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="X29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="Y29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="Z29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AA29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AB29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AC29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AD29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AE29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AF29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AG29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AH29" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="AI29" s="4" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="AJ29" s="11"/>
-      <c r="AK29" s="14"/>
-      <c r="AL29" s="11"/>
+        <f>IFERROR(AI24/(AI24+AI25),"")</f>
+        <v/>
+      </c>
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="21"/>
+      <c r="AL29" s="18"/>
     </row>
     <row r="30" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C30" s="35"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="45"/>
-      <c r="M30" s="45"/>
-      <c r="N30" s="45"/>
-      <c r="O30" s="45"/>
-      <c r="P30" s="45"/>
-      <c r="Q30" s="45"/>
-      <c r="R30" s="45"/>
-      <c r="S30" s="45"/>
-      <c r="T30" s="45"/>
-      <c r="U30" s="45"/>
-      <c r="V30" s="45"/>
-      <c r="W30" s="45"/>
-      <c r="X30" s="45"/>
-      <c r="Y30" s="45"/>
-      <c r="Z30" s="45"/>
-      <c r="AA30" s="45"/>
-      <c r="AB30" s="45"/>
-      <c r="AC30" s="45"/>
-      <c r="AD30" s="45"/>
-      <c r="AE30" s="45"/>
-      <c r="AF30" s="45"/>
-      <c r="AG30" s="45"/>
-      <c r="AH30" s="45"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="7"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="7"/>
+      <c r="AC30" s="7"/>
+      <c r="AD30" s="7"/>
+      <c r="AE30" s="7"/>
+      <c r="AF30" s="7"/>
+      <c r="AG30" s="7"/>
+      <c r="AH30" s="7"/>
       <c r="AI30" s="8">
-        <f t="shared" ref="AI30:AI35" si="12">SUM(D30:AH30)</f>
+        <f t="shared" ref="AI30:AI35" si="13">SUM(D30:AH30)</f>
         <v>0</v>
       </c>
-      <c r="AJ30" s="9"/>
-      <c r="AK30" s="12" t="str">
+      <c r="AJ30" s="16"/>
+      <c r="AK30" s="19" t="str">
         <f>IFERROR(AI30/AL30,"")</f>
         <v/>
       </c>
-      <c r="AL30" s="9"/>
+      <c r="AL30" s="16"/>
     </row>
     <row r="31" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A31" s="30"/>
-      <c r="B31" s="35" t="s">
+      <c r="A31" s="45"/>
+      <c r="B31" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C31" s="35"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="45"/>
-      <c r="M31" s="45"/>
-      <c r="N31" s="45"/>
-      <c r="O31" s="45"/>
-      <c r="P31" s="45"/>
-      <c r="Q31" s="45"/>
-      <c r="R31" s="45"/>
-      <c r="S31" s="45"/>
-      <c r="T31" s="45"/>
-      <c r="U31" s="45"/>
-      <c r="V31" s="45"/>
-      <c r="W31" s="45"/>
-      <c r="X31" s="45"/>
-      <c r="Y31" s="45"/>
-      <c r="Z31" s="45"/>
-      <c r="AA31" s="45"/>
-      <c r="AB31" s="45"/>
-      <c r="AC31" s="45"/>
-      <c r="AD31" s="45"/>
-      <c r="AE31" s="45"/>
-      <c r="AF31" s="45"/>
-      <c r="AG31" s="45"/>
-      <c r="AH31" s="45"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7"/>
+      <c r="AC31" s="7"/>
+      <c r="AD31" s="7"/>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
       <c r="AI31" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AJ31" s="10"/>
-      <c r="AK31" s="13"/>
-      <c r="AL31" s="10"/>
+      <c r="AJ31" s="17"/>
+      <c r="AK31" s="20"/>
+      <c r="AL31" s="17"/>
     </row>
     <row r="32" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A32" s="30"/>
-      <c r="B32" s="32" t="s">
+      <c r="A32" s="45"/>
+      <c r="B32" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="44" t="s">
+      <c r="C32" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D32" s="45"/>
-      <c r="E32" s="45"/>
-      <c r="F32" s="45"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="45"/>
-      <c r="I32" s="45"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="45"/>
-      <c r="M32" s="45"/>
-      <c r="N32" s="45"/>
-      <c r="O32" s="45"/>
-      <c r="P32" s="45"/>
-      <c r="Q32" s="45"/>
-      <c r="R32" s="45"/>
-      <c r="S32" s="45"/>
-      <c r="T32" s="45"/>
-      <c r="U32" s="45"/>
-      <c r="V32" s="45"/>
-      <c r="W32" s="45"/>
-      <c r="X32" s="45"/>
-      <c r="Y32" s="45"/>
-      <c r="Z32" s="45"/>
-      <c r="AA32" s="45"/>
-      <c r="AB32" s="45"/>
-      <c r="AC32" s="45"/>
-      <c r="AD32" s="45"/>
-      <c r="AE32" s="45"/>
-      <c r="AF32" s="45"/>
-      <c r="AG32" s="45"/>
-      <c r="AH32" s="45"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="7"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="7"/>
+      <c r="Q32" s="7"/>
+      <c r="R32" s="7"/>
+      <c r="S32" s="7"/>
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="7"/>
+      <c r="Z32" s="7"/>
+      <c r="AA32" s="7"/>
+      <c r="AB32" s="7"/>
+      <c r="AC32" s="7"/>
+      <c r="AD32" s="7"/>
+      <c r="AE32" s="7"/>
+      <c r="AF32" s="7"/>
+      <c r="AG32" s="7"/>
+      <c r="AH32" s="7"/>
       <c r="AI32" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AJ32" s="10"/>
-      <c r="AK32" s="13"/>
-      <c r="AL32" s="10"/>
+      <c r="AJ32" s="17"/>
+      <c r="AK32" s="20"/>
+      <c r="AL32" s="17"/>
     </row>
     <row r="33" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A33" s="30"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="31" t="s">
+      <c r="A33" s="45"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D33" s="45"/>
-      <c r="E33" s="45"/>
-      <c r="F33" s="45"/>
-      <c r="G33" s="45"/>
-      <c r="H33" s="45"/>
-      <c r="I33" s="45"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="45"/>
-      <c r="M33" s="45"/>
-      <c r="N33" s="45"/>
-      <c r="O33" s="45"/>
-      <c r="P33" s="45"/>
-      <c r="Q33" s="45"/>
-      <c r="R33" s="45"/>
-      <c r="S33" s="45"/>
-      <c r="T33" s="45"/>
-      <c r="U33" s="45"/>
-      <c r="V33" s="45"/>
-      <c r="W33" s="45"/>
-      <c r="X33" s="45"/>
-      <c r="Y33" s="45"/>
-      <c r="Z33" s="45"/>
-      <c r="AA33" s="45"/>
-      <c r="AB33" s="45"/>
-      <c r="AC33" s="45"/>
-      <c r="AD33" s="45"/>
-      <c r="AE33" s="45"/>
-      <c r="AF33" s="45"/>
-      <c r="AG33" s="45"/>
-      <c r="AH33" s="45"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7"/>
+      <c r="AC33" s="7"/>
+      <c r="AD33" s="7"/>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
       <c r="AI33" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AJ33" s="10"/>
-      <c r="AK33" s="13"/>
-      <c r="AL33" s="10"/>
+      <c r="AJ33" s="17"/>
+      <c r="AK33" s="20"/>
+      <c r="AL33" s="17"/>
     </row>
     <row r="34" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A34" s="30"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="31" t="s">
+      <c r="A34" s="45"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="D34" s="45"/>
-      <c r="E34" s="45"/>
-      <c r="F34" s="45"/>
-      <c r="G34" s="45"/>
-      <c r="H34" s="45"/>
-      <c r="I34" s="45"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="45"/>
-      <c r="M34" s="45"/>
-      <c r="N34" s="45"/>
-      <c r="O34" s="45"/>
-      <c r="P34" s="45"/>
-      <c r="Q34" s="45"/>
-      <c r="R34" s="45"/>
-      <c r="S34" s="45"/>
-      <c r="T34" s="45"/>
-      <c r="U34" s="45"/>
-      <c r="V34" s="45"/>
-      <c r="W34" s="45"/>
-      <c r="X34" s="45"/>
-      <c r="Y34" s="45"/>
-      <c r="Z34" s="45"/>
-      <c r="AA34" s="45"/>
-      <c r="AB34" s="45"/>
-      <c r="AC34" s="45"/>
-      <c r="AD34" s="45"/>
-      <c r="AE34" s="45"/>
-      <c r="AF34" s="45"/>
-      <c r="AG34" s="45"/>
-      <c r="AH34" s="45"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
+      <c r="AB34" s="7"/>
+      <c r="AC34" s="7"/>
+      <c r="AD34" s="7"/>
+      <c r="AE34" s="7"/>
+      <c r="AF34" s="7"/>
+      <c r="AG34" s="7"/>
+      <c r="AH34" s="7"/>
       <c r="AI34" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AJ34" s="10"/>
-      <c r="AK34" s="13"/>
-      <c r="AL34" s="10"/>
+      <c r="AJ34" s="17"/>
+      <c r="AK34" s="20"/>
+      <c r="AL34" s="17"/>
     </row>
     <row r="35" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A35" s="30"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="31" t="s">
+      <c r="A35" s="45"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="45"/>
-      <c r="G35" s="45"/>
-      <c r="H35" s="45"/>
-      <c r="I35" s="45"/>
-      <c r="J35" s="45"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="45"/>
-      <c r="M35" s="45"/>
-      <c r="N35" s="45"/>
-      <c r="O35" s="45"/>
-      <c r="P35" s="45"/>
-      <c r="Q35" s="45"/>
-      <c r="R35" s="45"/>
-      <c r="S35" s="45"/>
-      <c r="T35" s="45"/>
-      <c r="U35" s="45"/>
-      <c r="V35" s="45"/>
-      <c r="W35" s="45"/>
-      <c r="X35" s="45"/>
-      <c r="Y35" s="45"/>
-      <c r="Z35" s="45"/>
-      <c r="AA35" s="45"/>
-      <c r="AB35" s="45"/>
-      <c r="AC35" s="45"/>
-      <c r="AD35" s="45"/>
-      <c r="AE35" s="45"/>
-      <c r="AF35" s="45"/>
-      <c r="AG35" s="45"/>
-      <c r="AH35" s="45"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7"/>
+      <c r="AC35" s="7"/>
+      <c r="AD35" s="7"/>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
       <c r="AI35" s="8">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AJ35" s="10"/>
-      <c r="AK35" s="13"/>
-      <c r="AL35" s="10"/>
+      <c r="AJ35" s="17"/>
+      <c r="AK35" s="20"/>
+      <c r="AL35" s="17"/>
     </row>
     <row r="36" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A36" s="30"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="31" t="s">
+      <c r="A36" s="45"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45"/>
-      <c r="T36" s="45"/>
-      <c r="U36" s="45"/>
-      <c r="V36" s="45"/>
-      <c r="W36" s="45"/>
-      <c r="X36" s="45"/>
-      <c r="Y36" s="45"/>
-      <c r="Z36" s="45"/>
-      <c r="AA36" s="45"/>
-      <c r="AB36" s="45"/>
-      <c r="AC36" s="45"/>
-      <c r="AD36" s="45"/>
-      <c r="AE36" s="45"/>
-      <c r="AF36" s="45"/>
-      <c r="AG36" s="45"/>
-      <c r="AH36" s="45"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="7"/>
+      <c r="AB36" s="7"/>
+      <c r="AC36" s="7"/>
+      <c r="AD36" s="7"/>
+      <c r="AE36" s="7"/>
+      <c r="AF36" s="7"/>
+      <c r="AG36" s="7"/>
+      <c r="AH36" s="7"/>
       <c r="AI36" s="8">
-        <f t="shared" ref="AI36" si="13">SUM(D36:AH36)</f>
+        <f t="shared" ref="AI36" si="14">SUM(D36:AH36)</f>
         <v>0</v>
       </c>
-      <c r="AJ36" s="10"/>
-      <c r="AK36" s="13"/>
-      <c r="AL36" s="10"/>
+      <c r="AJ36" s="17"/>
+      <c r="AK36" s="20"/>
+      <c r="AL36" s="17"/>
     </row>
     <row r="37" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A37" s="30"/>
-      <c r="B37" s="42" t="s">
+      <c r="A37" s="45"/>
+      <c r="B37" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="42"/>
+      <c r="C37" s="28"/>
       <c r="D37" s="4" t="str">
-        <f>IFERROR(D35/(D35+D36),"")</f>
+        <f>IFERROR(D30/(D30+D31),"")</f>
         <v/>
       </c>
       <c r="E37" s="4" t="str">
-        <f t="shared" ref="E37:AI37" si="14">IFERROR(E35/(E35+E36),"")</f>
+        <f t="shared" ref="E37:AH37" si="15">IFERROR(E30/(E30+E31),"")</f>
         <v/>
       </c>
       <c r="F37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="G37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="H37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="I37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="J37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="K37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="L37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="M37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="N37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="O37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="P37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Q37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="R37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="S37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="T37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="U37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="V37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="W37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="X37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Y37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="Z37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AA37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AB37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AC37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AD37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AE37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AF37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AG37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AH37" s="4" t="str">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v/>
       </c>
       <c r="AI37" s="4" t="str">
-        <f t="shared" si="14"/>
-        <v/>
-      </c>
-      <c r="AJ37" s="11"/>
-      <c r="AK37" s="14"/>
-      <c r="AL37" s="11"/>
+        <f>IFERROR(AI30/(AI30+AI31),"")</f>
+        <v/>
+      </c>
+      <c r="AJ37" s="18"/>
+      <c r="AK37" s="21"/>
+      <c r="AL37" s="18"/>
     </row>
     <row r="38" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="35" t="s">
+      <c r="B38" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C38" s="35"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="45"/>
-      <c r="G38" s="45"/>
-      <c r="H38" s="45"/>
-      <c r="I38" s="45"/>
-      <c r="J38" s="45"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="45"/>
-      <c r="M38" s="45"/>
-      <c r="N38" s="45"/>
-      <c r="O38" s="45"/>
-      <c r="P38" s="45"/>
-      <c r="Q38" s="45"/>
-      <c r="R38" s="45"/>
-      <c r="S38" s="45"/>
-      <c r="T38" s="45"/>
-      <c r="U38" s="45"/>
-      <c r="V38" s="45"/>
-      <c r="W38" s="45"/>
-      <c r="X38" s="45"/>
-      <c r="Y38" s="45"/>
-      <c r="Z38" s="45"/>
-      <c r="AA38" s="45"/>
-      <c r="AB38" s="45"/>
-      <c r="AC38" s="45"/>
-      <c r="AD38" s="45"/>
-      <c r="AE38" s="45"/>
-      <c r="AF38" s="45"/>
-      <c r="AG38" s="45"/>
-      <c r="AH38" s="45"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
+      <c r="K38" s="7"/>
+      <c r="L38" s="7"/>
+      <c r="M38" s="7"/>
+      <c r="N38" s="7"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="7"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
+      <c r="S38" s="7"/>
+      <c r="T38" s="7"/>
+      <c r="U38" s="7"/>
+      <c r="V38" s="7"/>
+      <c r="W38" s="7"/>
+      <c r="X38" s="7"/>
+      <c r="Y38" s="7"/>
+      <c r="Z38" s="7"/>
+      <c r="AA38" s="7"/>
+      <c r="AB38" s="7"/>
+      <c r="AC38" s="7"/>
+      <c r="AD38" s="7"/>
+      <c r="AE38" s="7"/>
+      <c r="AF38" s="7"/>
+      <c r="AG38" s="7"/>
+      <c r="AH38" s="7"/>
       <c r="AI38" s="8">
-        <f t="shared" ref="AI38:AI43" si="15">SUM(D38:AH38)</f>
+        <f t="shared" ref="AI38:AI43" si="16">SUM(D38:AH38)</f>
         <v>0</v>
       </c>
-      <c r="AJ38" s="9"/>
-      <c r="AK38" s="12" t="str">
+      <c r="AJ38" s="16"/>
+      <c r="AK38" s="19" t="str">
         <f>IFERROR(AI38/AL38,"")</f>
         <v/>
       </c>
-      <c r="AL38" s="9"/>
+      <c r="AL38" s="16"/>
     </row>
     <row r="39" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A39" s="30"/>
-      <c r="B39" s="35" t="s">
+      <c r="A39" s="45"/>
+      <c r="B39" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="C39" s="35"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="45"/>
-      <c r="G39" s="45"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="45"/>
-      <c r="R39" s="45"/>
-      <c r="S39" s="45"/>
-      <c r="T39" s="45"/>
-      <c r="U39" s="45"/>
-      <c r="V39" s="45"/>
-      <c r="W39" s="45"/>
-      <c r="X39" s="45"/>
-      <c r="Y39" s="45"/>
-      <c r="Z39" s="45"/>
-      <c r="AA39" s="45"/>
-      <c r="AB39" s="45"/>
-      <c r="AC39" s="45"/>
-      <c r="AD39" s="45"/>
-      <c r="AE39" s="45"/>
-      <c r="AF39" s="45"/>
-      <c r="AG39" s="45"/>
-      <c r="AH39" s="45"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
+      <c r="L39" s="7"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="7"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
+      <c r="S39" s="7"/>
+      <c r="T39" s="7"/>
+      <c r="U39" s="7"/>
+      <c r="V39" s="7"/>
+      <c r="W39" s="7"/>
+      <c r="X39" s="7"/>
+      <c r="Y39" s="7"/>
+      <c r="Z39" s="7"/>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7"/>
+      <c r="AC39" s="7"/>
+      <c r="AD39" s="7"/>
+      <c r="AE39" s="7"/>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
       <c r="AI39" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AJ39" s="10"/>
-      <c r="AK39" s="13"/>
-      <c r="AL39" s="10"/>
+      <c r="AJ39" s="17"/>
+      <c r="AK39" s="20"/>
+      <c r="AL39" s="17"/>
     </row>
     <row r="40" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A40" s="30"/>
-      <c r="B40" s="32" t="s">
+      <c r="A40" s="45"/>
+      <c r="B40" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="C40" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="45"/>
-      <c r="G40" s="45"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="45"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="45"/>
-      <c r="M40" s="45"/>
-      <c r="N40" s="45"/>
-      <c r="O40" s="45"/>
-      <c r="P40" s="45"/>
-      <c r="Q40" s="45"/>
-      <c r="R40" s="45"/>
-      <c r="S40" s="45"/>
-      <c r="T40" s="45"/>
-      <c r="U40" s="45"/>
-      <c r="V40" s="45"/>
-      <c r="W40" s="45"/>
-      <c r="X40" s="45"/>
-      <c r="Y40" s="45"/>
-      <c r="Z40" s="45"/>
-      <c r="AA40" s="45"/>
-      <c r="AB40" s="45"/>
-      <c r="AC40" s="45"/>
-      <c r="AD40" s="45"/>
-      <c r="AE40" s="45"/>
-      <c r="AF40" s="45"/>
-      <c r="AG40" s="45"/>
-      <c r="AH40" s="45"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="7"/>
+      <c r="L40" s="7"/>
+      <c r="M40" s="7"/>
+      <c r="N40" s="7"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="7"/>
+      <c r="Q40" s="7"/>
+      <c r="R40" s="7"/>
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="7"/>
+      <c r="W40" s="7"/>
+      <c r="X40" s="7"/>
+      <c r="Y40" s="7"/>
+      <c r="Z40" s="7"/>
+      <c r="AA40" s="7"/>
+      <c r="AB40" s="7"/>
+      <c r="AC40" s="7"/>
+      <c r="AD40" s="7"/>
+      <c r="AE40" s="7"/>
+      <c r="AF40" s="7"/>
+      <c r="AG40" s="7"/>
+      <c r="AH40" s="7"/>
       <c r="AI40" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AJ40" s="10"/>
-      <c r="AK40" s="13"/>
-      <c r="AL40" s="10"/>
+      <c r="AJ40" s="17"/>
+      <c r="AK40" s="20"/>
+      <c r="AL40" s="17"/>
     </row>
     <row r="41" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A41" s="30"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="31" t="s">
+      <c r="A41" s="45"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="45"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="45"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="45"/>
-      <c r="M41" s="45"/>
-      <c r="N41" s="45"/>
-      <c r="O41" s="45"/>
-      <c r="P41" s="45"/>
-      <c r="Q41" s="45"/>
-      <c r="R41" s="45"/>
-      <c r="S41" s="45"/>
-      <c r="T41" s="45"/>
-      <c r="U41" s="45"/>
-      <c r="V41" s="45"/>
-      <c r="W41" s="45"/>
-      <c r="X41" s="45"/>
-      <c r="Y41" s="45"/>
-      <c r="Z41" s="45"/>
-      <c r="AA41" s="45"/>
-      <c r="AB41" s="45"/>
-      <c r="AC41" s="45"/>
-      <c r="AD41" s="45"/>
-      <c r="AE41" s="45"/>
-      <c r="AF41" s="45"/>
-      <c r="AG41" s="45"/>
-      <c r="AH41" s="45"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
+      <c r="K41" s="7"/>
+      <c r="L41" s="7"/>
+      <c r="M41" s="7"/>
+      <c r="N41" s="7"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="7"/>
+      <c r="Z41" s="7"/>
+      <c r="AA41" s="7"/>
+      <c r="AB41" s="7"/>
+      <c r="AC41" s="7"/>
+      <c r="AD41" s="7"/>
+      <c r="AE41" s="7"/>
+      <c r="AF41" s="7"/>
+      <c r="AG41" s="7"/>
+      <c r="AH41" s="7"/>
       <c r="AI41" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AJ41" s="10"/>
-      <c r="AK41" s="13"/>
-      <c r="AL41" s="10"/>
+      <c r="AJ41" s="17"/>
+      <c r="AK41" s="20"/>
+      <c r="AL41" s="17"/>
     </row>
     <row r="42" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A42" s="30"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="31" t="s">
+      <c r="A42" s="45"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="45"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="45"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="45"/>
-      <c r="M42" s="45"/>
-      <c r="N42" s="45"/>
-      <c r="O42" s="45"/>
-      <c r="P42" s="45"/>
-      <c r="Q42" s="45"/>
-      <c r="R42" s="45"/>
-      <c r="S42" s="45"/>
-      <c r="T42" s="45"/>
-      <c r="U42" s="45"/>
-      <c r="V42" s="45"/>
-      <c r="W42" s="45"/>
-      <c r="X42" s="45"/>
-      <c r="Y42" s="45"/>
-      <c r="Z42" s="45"/>
-      <c r="AA42" s="45"/>
-      <c r="AB42" s="45"/>
-      <c r="AC42" s="45"/>
-      <c r="AD42" s="45"/>
-      <c r="AE42" s="45"/>
-      <c r="AF42" s="45"/>
-      <c r="AG42" s="45"/>
-      <c r="AH42" s="45"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
+      <c r="K42" s="7"/>
+      <c r="L42" s="7"/>
+      <c r="M42" s="7"/>
+      <c r="N42" s="7"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="7"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
+      <c r="S42" s="7"/>
+      <c r="T42" s="7"/>
+      <c r="U42" s="7"/>
+      <c r="V42" s="7"/>
+      <c r="W42" s="7"/>
+      <c r="X42" s="7"/>
+      <c r="Y42" s="7"/>
+      <c r="Z42" s="7"/>
+      <c r="AA42" s="7"/>
+      <c r="AB42" s="7"/>
+      <c r="AC42" s="7"/>
+      <c r="AD42" s="7"/>
+      <c r="AE42" s="7"/>
+      <c r="AF42" s="7"/>
+      <c r="AG42" s="7"/>
+      <c r="AH42" s="7"/>
       <c r="AI42" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AJ42" s="10"/>
-      <c r="AK42" s="13"/>
-      <c r="AL42" s="10"/>
+      <c r="AJ42" s="17"/>
+      <c r="AK42" s="20"/>
+      <c r="AL42" s="17"/>
     </row>
     <row r="43" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A43" s="30"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="31" t="s">
+      <c r="A43" s="45"/>
+      <c r="B43" s="47"/>
+      <c r="C43" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="45"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="45"/>
-      <c r="I43" s="45"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="45"/>
-      <c r="M43" s="45"/>
-      <c r="N43" s="45"/>
-      <c r="O43" s="45"/>
-      <c r="P43" s="45"/>
-      <c r="Q43" s="45"/>
-      <c r="R43" s="45"/>
-      <c r="S43" s="45"/>
-      <c r="T43" s="45"/>
-      <c r="U43" s="45"/>
-      <c r="V43" s="45"/>
-      <c r="W43" s="45"/>
-      <c r="X43" s="45"/>
-      <c r="Y43" s="45"/>
-      <c r="Z43" s="45"/>
-      <c r="AA43" s="45"/>
-      <c r="AB43" s="45"/>
-      <c r="AC43" s="45"/>
-      <c r="AD43" s="45"/>
-      <c r="AE43" s="45"/>
-      <c r="AF43" s="45"/>
-      <c r="AG43" s="45"/>
-      <c r="AH43" s="45"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="7"/>
+      <c r="L43" s="7"/>
+      <c r="M43" s="7"/>
+      <c r="N43" s="7"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="7"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
+      <c r="S43" s="7"/>
+      <c r="T43" s="7"/>
+      <c r="U43" s="7"/>
+      <c r="V43" s="7"/>
+      <c r="W43" s="7"/>
+      <c r="X43" s="7"/>
+      <c r="Y43" s="7"/>
+      <c r="Z43" s="7"/>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="7"/>
+      <c r="AC43" s="7"/>
+      <c r="AD43" s="7"/>
+      <c r="AE43" s="7"/>
+      <c r="AF43" s="7"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
       <c r="AI43" s="8">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
-      <c r="AJ43" s="10"/>
-      <c r="AK43" s="13"/>
-      <c r="AL43" s="10"/>
+      <c r="AJ43" s="17"/>
+      <c r="AK43" s="20"/>
+      <c r="AL43" s="17"/>
     </row>
     <row r="44" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A44" s="30"/>
-      <c r="B44" s="42" t="s">
+      <c r="A44" s="45"/>
+      <c r="B44" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C44" s="42"/>
+      <c r="C44" s="28"/>
       <c r="D44" s="4" t="str">
-        <f>IFERROR(D42/(D42+D43),"")</f>
+        <f>IFERROR(D38/(D38+D39),"")</f>
         <v/>
       </c>
       <c r="E44" s="4" t="str">
-        <f t="shared" ref="E44:AI44" si="16">IFERROR(E42/(E42+E43),"")</f>
+        <f t="shared" ref="E44:AH44" si="17">IFERROR(E38/(E38+E39),"")</f>
         <v/>
       </c>
       <c r="F44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="G44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="H44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="I44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="J44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="K44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="L44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="M44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="N44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="O44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="P44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="Q44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="R44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="S44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="T44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="U44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="V44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="W44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="X44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="Y44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="Z44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AA44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AB44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AC44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AD44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AE44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AF44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AG44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AH44" s="4" t="str">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v/>
       </c>
       <c r="AI44" s="4" t="str">
-        <f t="shared" si="16"/>
-        <v/>
-      </c>
-      <c r="AJ44" s="11"/>
-      <c r="AK44" s="14"/>
-      <c r="AL44" s="11"/>
+        <f>IFERROR(AI38/(AI38+AI39),"")</f>
+        <v/>
+      </c>
+      <c r="AJ44" s="18"/>
+      <c r="AK44" s="21"/>
+      <c r="AL44" s="18"/>
     </row>
     <row r="45" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A45" s="33" t="s">
+      <c r="A45" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C45" s="35"/>
+      <c r="C45" s="31"/>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
@@ -3963,22 +3957,22 @@
       <c r="AG45" s="7"/>
       <c r="AH45" s="7"/>
       <c r="AI45" s="8">
-        <f t="shared" ref="AI45:AI46" si="17">SUM(D45:AH45)</f>
+        <f t="shared" ref="AI45:AI46" si="18">SUM(D45:AH45)</f>
         <v>0</v>
       </c>
-      <c r="AJ45" s="9"/>
-      <c r="AK45" s="47" t="str">
-        <f t="shared" ref="AK45" si="18">IFERROR(AI45/AL45,"")</f>
-        <v/>
-      </c>
-      <c r="AL45" s="9"/>
+      <c r="AJ45" s="16"/>
+      <c r="AK45" s="22" t="str">
+        <f t="shared" ref="AK45" si="19">IFERROR(AI45/AL45,"")</f>
+        <v/>
+      </c>
+      <c r="AL45" s="16"/>
     </row>
     <row r="46" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A46" s="39"/>
-      <c r="B46" s="43" t="s">
+      <c r="A46" s="41"/>
+      <c r="B46" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="43"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -4011,198 +4005,198 @@
       <c r="AG46" s="7"/>
       <c r="AH46" s="7"/>
       <c r="AI46" s="8">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
-      <c r="AJ46" s="10"/>
-      <c r="AK46" s="47"/>
-      <c r="AL46" s="10"/>
+      <c r="AJ46" s="17"/>
+      <c r="AK46" s="22"/>
+      <c r="AL46" s="17"/>
     </row>
     <row r="47" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A47" s="39"/>
-      <c r="B47" s="42" t="s">
+      <c r="A47" s="41"/>
+      <c r="B47" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C47" s="42"/>
+      <c r="C47" s="28"/>
       <c r="D47" s="4" t="str">
         <f>IFERROR(D45/(D45+D46),"")</f>
         <v/>
       </c>
       <c r="E47" s="4" t="str">
-        <f t="shared" ref="E47:AI47" si="19">IFERROR(E45/(E45+E46),"")</f>
+        <f t="shared" ref="E47:AH47" si="20">IFERROR(E45/(E45+E46),"")</f>
         <v/>
       </c>
       <c r="F47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="G47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="H47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="I47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="J47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="K47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="L47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="M47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="N47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="O47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="P47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="Q47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="R47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="S47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="T47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="U47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="V47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="W47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="X47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="Y47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="Z47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AA47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AB47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AC47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AD47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AE47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AF47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AG47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AH47" s="4" t="str">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v/>
       </c>
       <c r="AI47" s="4" t="str">
-        <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="AJ47" s="11"/>
-      <c r="AK47" s="47"/>
-      <c r="AL47" s="11"/>
+        <f>IFERROR(AI45/(AI45+AI46),"")</f>
+        <v/>
+      </c>
+      <c r="AJ47" s="18"/>
+      <c r="AK47" s="22"/>
+      <c r="AL47" s="18"/>
     </row>
     <row r="48" spans="1:38" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="B48" s="16"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
-      <c r="E48" s="16"/>
-      <c r="F48" s="16"/>
-      <c r="G48" s="16"/>
-      <c r="H48" s="16"/>
-      <c r="I48" s="16"/>
-      <c r="J48" s="16"/>
-      <c r="K48" s="16"/>
-      <c r="L48" s="16"/>
-      <c r="M48" s="16"/>
-      <c r="N48" s="16"/>
-      <c r="O48" s="16"/>
-      <c r="P48" s="16"/>
-      <c r="Q48" s="16"/>
-      <c r="R48" s="16"/>
-      <c r="S48" s="16"/>
-      <c r="T48" s="16"/>
-      <c r="U48" s="16"/>
-      <c r="V48" s="16"/>
-      <c r="W48" s="16"/>
-      <c r="X48" s="16"/>
-      <c r="Y48" s="16"/>
-      <c r="Z48" s="16"/>
-      <c r="AA48" s="16"/>
-      <c r="AB48" s="16"/>
-      <c r="AC48" s="16"/>
-      <c r="AD48" s="16"/>
-      <c r="AE48" s="16"/>
-      <c r="AF48" s="16"/>
-      <c r="AG48" s="16"/>
-      <c r="AH48" s="17"/>
-      <c r="AI48" s="5">
-        <f>IFERROR(PRODUCT(AI4,AI7,AI16,AI23,AI29,AI37,AI44,AI47),"")</f>
-        <v>0</v>
+      <c r="B48" s="35"/>
+      <c r="C48" s="35"/>
+      <c r="D48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="35"/>
+      <c r="H48" s="35"/>
+      <c r="I48" s="35"/>
+      <c r="J48" s="35"/>
+      <c r="K48" s="35"/>
+      <c r="L48" s="35"/>
+      <c r="M48" s="35"/>
+      <c r="N48" s="35"/>
+      <c r="O48" s="35"/>
+      <c r="P48" s="35"/>
+      <c r="Q48" s="35"/>
+      <c r="R48" s="35"/>
+      <c r="S48" s="35"/>
+      <c r="T48" s="35"/>
+      <c r="U48" s="35"/>
+      <c r="V48" s="35"/>
+      <c r="W48" s="35"/>
+      <c r="X48" s="35"/>
+      <c r="Y48" s="35"/>
+      <c r="Z48" s="35"/>
+      <c r="AA48" s="35"/>
+      <c r="AB48" s="35"/>
+      <c r="AC48" s="35"/>
+      <c r="AD48" s="35"/>
+      <c r="AE48" s="35"/>
+      <c r="AF48" s="35"/>
+      <c r="AG48" s="35"/>
+      <c r="AH48" s="36"/>
+      <c r="AI48" s="5" t="str">
+        <f>IFERROR(AVERAGE(AI4,AI7,AI16,AI23,AI29,AI37,AI44,AI47),"")</f>
+        <v/>
       </c>
       <c r="AJ48" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="AK48" s="5">
-        <f>IFERROR(PRODUCT(AK2,AK5,AK8,AK17,AK30,AK24,AK38,AK45),"")</f>
-        <v>0</v>
+      <c r="AK48" s="5" t="str">
+        <f>IFERROR(AVERAGE(AK2,AK5,AK8,AK17,AK24,AK30,AK38,AK45),"")</f>
+        <v/>
       </c>
       <c r="AL48" s="6" t="s">
         <v>9</v>
@@ -4210,41 +4204,12 @@
     </row>
   </sheetData>
   <mergeCells count="57">
-    <mergeCell ref="AJ38:AJ44"/>
-    <mergeCell ref="AK38:AK44"/>
-    <mergeCell ref="AL38:AL44"/>
-    <mergeCell ref="AJ45:AJ47"/>
-    <mergeCell ref="AK45:AK47"/>
-    <mergeCell ref="AL45:AL47"/>
-    <mergeCell ref="AJ8:AJ16"/>
-    <mergeCell ref="AK8:AK16"/>
-    <mergeCell ref="AL8:AL16"/>
-    <mergeCell ref="AJ17:AJ23"/>
-    <mergeCell ref="AK17:AK23"/>
-    <mergeCell ref="AL17:AL23"/>
-    <mergeCell ref="AJ24:AJ29"/>
-    <mergeCell ref="AK24:AK29"/>
-    <mergeCell ref="AL24:AL29"/>
-    <mergeCell ref="AJ30:AJ37"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="AK30:AK37"/>
-    <mergeCell ref="AL30:AL37"/>
-    <mergeCell ref="AK2:AK4"/>
-    <mergeCell ref="AK5:AK7"/>
-    <mergeCell ref="AL2:AL4"/>
-    <mergeCell ref="AL5:AL7"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B19:B22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="AJ2:AJ4"/>
-    <mergeCell ref="AJ5:AJ7"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:B36"/>
+    <mergeCell ref="B40:B43"/>
     <mergeCell ref="A48:AH48"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:A7"/>
@@ -4261,12 +4226,41 @@
     <mergeCell ref="B44:C44"/>
     <mergeCell ref="B38:C38"/>
     <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B32:B36"/>
-    <mergeCell ref="B40:B43"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="AK2:AK4"/>
+    <mergeCell ref="AK5:AK7"/>
+    <mergeCell ref="AL2:AL4"/>
+    <mergeCell ref="AL5:AL7"/>
+    <mergeCell ref="C2:C4"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="AJ2:AJ4"/>
+    <mergeCell ref="AJ5:AJ7"/>
+    <mergeCell ref="AJ24:AJ29"/>
+    <mergeCell ref="AK24:AK29"/>
+    <mergeCell ref="AL24:AL29"/>
+    <mergeCell ref="AJ30:AJ37"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="AK30:AK37"/>
+    <mergeCell ref="AL30:AL37"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="AJ8:AJ16"/>
+    <mergeCell ref="AK8:AK16"/>
+    <mergeCell ref="AL8:AL16"/>
+    <mergeCell ref="AJ17:AJ23"/>
+    <mergeCell ref="AK17:AK23"/>
+    <mergeCell ref="AL17:AL23"/>
+    <mergeCell ref="AJ38:AJ44"/>
+    <mergeCell ref="AK38:AK44"/>
+    <mergeCell ref="AL38:AL44"/>
+    <mergeCell ref="AJ45:AJ47"/>
+    <mergeCell ref="AK45:AK47"/>
+    <mergeCell ref="AL45:AL47"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>